<commit_message>
modify car action logic.
</commit_message>
<xml_diff>
--- a/docs/address-2018-4-17.xlsx
+++ b/docs/address-2018-4-17.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FE4F9A86-5A82-418A-AFEC-CBCD7D3F5D84}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{57236C60-8996-4E78-AD01-F641A2F75B1B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="机械手动作地址" sheetId="1" r:id="rId1"/>
@@ -2483,8 +2483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3412,8 +3412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4361,7 +4361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>

</xml_diff>